<commit_message>
automation project with selenium webdriver for rokomari.com
</commit_message>
<xml_diff>
--- a/TestCase for Rokomari (Signin To Checkout).xlsx
+++ b/TestCase for Rokomari (Signin To Checkout).xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shovon\Desktop\New folder (4)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Training Program\SQA\Hands On SQA and Cyber Security\Assignment\Automation Testing\Automation Project with Selenium WebDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B23061D-8FC8-42E4-B1AA-D1F7420358F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8663E23-CDFA-4C9E-B4FB-C529FDC714D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5865" xr2:uid="{9B6C14D2-D88D-4551-9CFD-A50D6C9631AA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="140">
   <si>
     <t>Product Name</t>
   </si>
@@ -318,18 +318,6 @@
 2. Click on "Sign in" option
 3. Now enter invalid email and valid password
 4. Click on "Sign in" button</t>
-  </si>
-  <si>
-    <t>email: 
-abcd@gmail.com
-password: 
-12345</t>
-  </si>
-  <si>
-    <t>email: 
-abcd@gmail.com
-password: 
-Rokomari@01</t>
   </si>
   <si>
     <t>email: 
@@ -518,6 +506,21 @@
   </si>
   <si>
     <t>Add To Cart</t>
+  </si>
+  <si>
+    <t>email: 
+efgh@gmail.com
+password: 
+12345</t>
+  </si>
+  <si>
+    <t>email: 
+efgh@gmail.com
+password: 
+Rokomari@01</t>
+  </si>
+  <si>
+    <t>Warning message with the text "Wrong email or phone efgh@gmail.com" should be displayed.</t>
   </si>
 </sst>
 </file>
@@ -1716,49 +1719,214 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="51" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="43" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="13" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1831,171 +1999,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="43" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="51" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4700,7 +4703,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4724,42 +4727,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="156" t="s">
-        <v>108</v>
-      </c>
-      <c r="D1" s="157"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="75"/>
       <c r="E1" s="44" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G1" s="1"/>
       <c r="M1" s="39"/>
-      <c r="N1" s="75" t="s">
+      <c r="N1" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="76"/>
+      <c r="O1" s="73"/>
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="71"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="77"/>
       <c r="E2" s="45" t="s">
         <v>24</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G2" s="1"/>
       <c r="M2" s="39"/>
@@ -4773,19 +4776,19 @@
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="70" t="s">
+      <c r="B3" s="81"/>
+      <c r="C3" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="71"/>
+      <c r="D3" s="77"/>
       <c r="E3" s="45" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G3" s="1"/>
       <c r="M3" s="39"/>
@@ -4799,19 +4802,19 @@
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="70" t="s">
+      <c r="B4" s="81"/>
+      <c r="C4" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="71"/>
+      <c r="D4" s="77"/>
       <c r="E4" s="45" t="s">
         <v>26</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G4" s="1"/>
       <c r="M4" s="39"/>
@@ -4825,12 +4828,12 @@
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
       <c r="E5" s="46" t="s">
         <v>27</v>
       </c>
@@ -4886,9 +4889,9 @@
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="150"/>
-      <c r="E8" s="151"/>
-      <c r="F8" s="151"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
       <c r="G8" s="4"/>
       <c r="H8" s="34"/>
       <c r="I8" s="34"/>
@@ -4897,53 +4900,53 @@
       <c r="L8" s="34"/>
       <c r="M8" s="34"/>
       <c r="N8" s="5"/>
-      <c r="O8" s="152"/>
+      <c r="O8" s="68"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="153" t="s">
+      <c r="A9" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="154" t="s">
+      <c r="B9" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="154" t="s">
+      <c r="C9" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="154" t="s">
+      <c r="D9" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="154" t="s">
+      <c r="E9" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="154" t="s">
+      <c r="F9" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="154" t="s">
+      <c r="G9" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="154" t="s">
+      <c r="H9" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="154" t="s">
+      <c r="I9" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="154" t="s">
+      <c r="J9" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="K9" s="154" t="s">
+      <c r="K9" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="L9" s="154" t="s">
+      <c r="L9" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="M9" s="154" t="s">
+      <c r="M9" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="154" t="s">
+      <c r="N9" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="O9" s="155" t="s">
+      <c r="O9" s="71" t="s">
         <v>13</v>
       </c>
       <c r="P9" s="1"/>
@@ -4952,11 +4955,11 @@
       <c r="A10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="88" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="85" t="s">
         <v>109</v>
-      </c>
-      <c r="C10" s="65" t="s">
-        <v>111</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>43</v>
@@ -4989,8 +4992,8 @@
       <c r="A11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="73"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="86"/>
       <c r="D11" s="8" t="s">
         <v>43</v>
       </c>
@@ -5016,22 +5019,22 @@
       <c r="A12" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="73"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="86"/>
       <c r="D12" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F12" s="43" t="s">
-        <v>93</v>
+        <v>137</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>90</v>
       </c>
       <c r="H12" s="42" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="I12" s="35" t="s">
         <v>42</v>
@@ -5047,22 +5050,22 @@
       <c r="A13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="73"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="86"/>
       <c r="D13" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F13" s="43" t="s">
-        <v>94</v>
+        <v>138</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>92</v>
       </c>
       <c r="H13" s="42" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="I13" s="35" t="s">
         <v>42</v>
@@ -5076,19 +5079,19 @@
       <c r="A14" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="73"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="86"/>
       <c r="D14" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F14" s="43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H14" s="42" t="s">
         <v>91</v>
@@ -5106,22 +5109,22 @@
       <c r="A15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="73"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="86"/>
       <c r="D15" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F15" s="43" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" s="42" t="s">
         <v>101</v>
-      </c>
-      <c r="H15" s="42" t="s">
-        <v>103</v>
       </c>
       <c r="I15" s="35" t="s">
         <v>42</v>
@@ -5135,22 +5138,22 @@
       <c r="A16" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="64"/>
-      <c r="C16" s="73"/>
+      <c r="B16" s="88"/>
+      <c r="C16" s="86"/>
       <c r="D16" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="43" t="s">
+      <c r="H16" s="42" t="s">
         <v>105</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="H16" s="42" t="s">
-        <v>107</v>
       </c>
       <c r="I16" s="35" t="s">
         <v>42</v>
@@ -5166,21 +5169,21 @@
       <c r="A17" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="64"/>
-      <c r="C17" s="73" t="s">
-        <v>118</v>
+      <c r="B17" s="88"/>
+      <c r="C17" s="86" t="s">
+        <v>116</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E17" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H17" s="35" t="s">
         <v>112</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H17" s="35" t="s">
-        <v>114</v>
       </c>
       <c r="I17" s="35" t="s">
         <v>42</v>
@@ -5195,19 +5198,19 @@
       <c r="A18" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="64"/>
-      <c r="C18" s="74"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="87"/>
       <c r="D18" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E18" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" s="35" t="s">
         <v>115</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H18" s="35" t="s">
-        <v>117</v>
       </c>
       <c r="I18" s="35" t="s">
         <v>42</v>
@@ -5222,21 +5225,21 @@
       <c r="A19" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="64"/>
+      <c r="B19" s="88"/>
       <c r="C19" s="63" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E19" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H19" s="35" t="s">
         <v>119</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="H19" s="35" t="s">
-        <v>121</v>
       </c>
       <c r="I19" s="35" t="s">
         <v>42</v>
@@ -5250,21 +5253,21 @@
       <c r="A20" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="64"/>
-      <c r="C20" s="73" t="s">
-        <v>138</v>
+      <c r="B20" s="88"/>
+      <c r="C20" s="86" t="s">
+        <v>136</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="H20" s="35" t="s">
         <v>123</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="H20" s="35" t="s">
-        <v>125</v>
       </c>
       <c r="I20" s="35" t="s">
         <v>42</v>
@@ -5278,19 +5281,19 @@
       <c r="A21" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="64"/>
-      <c r="C21" s="74"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="87"/>
       <c r="D21" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E21" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H21" s="35" t="s">
         <v>126</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="H21" s="35" t="s">
-        <v>128</v>
       </c>
       <c r="I21" s="35" t="s">
         <v>42</v>
@@ -5305,19 +5308,19 @@
       <c r="A22" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="74"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="87"/>
       <c r="D22" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E22" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H22" s="35" t="s">
         <v>129</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H22" s="35" t="s">
-        <v>131</v>
       </c>
       <c r="I22" s="35" t="s">
         <v>42</v>
@@ -5331,19 +5334,19 @@
       <c r="A23" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="74"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="87"/>
       <c r="D23" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E23" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H23" s="35" t="s">
         <v>132</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="H23" s="35" t="s">
-        <v>134</v>
       </c>
       <c r="I23" s="35" t="s">
         <v>42</v>
@@ -5357,19 +5360,19 @@
       <c r="A24" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="74"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="87"/>
       <c r="D24" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E24" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H24" s="35" t="s">
         <v>135</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H24" s="35" t="s">
-        <v>137</v>
       </c>
       <c r="I24" s="35" t="s">
         <v>42</v>
@@ -5382,8 +5385,8 @@
     </row>
     <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
-      <c r="B25" s="148"/>
-      <c r="C25" s="149"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="65"/>
       <c r="D25" s="8"/>
       <c r="G25" s="3"/>
       <c r="J25" s="12"/>
@@ -5393,8 +5396,8 @@
     </row>
     <row r="26" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
-      <c r="B26" s="148"/>
-      <c r="C26" s="149"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="65"/>
       <c r="D26" s="8"/>
       <c r="G26" s="3"/>
       <c r="J26" s="12"/>
@@ -5402,8 +5405,8 @@
     </row>
     <row r="27" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
-      <c r="B27" s="148"/>
-      <c r="C27" s="149"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="65"/>
       <c r="D27" s="8"/>
       <c r="G27" s="3"/>
       <c r="J27" s="12"/>
@@ -5413,8 +5416,8 @@
     </row>
     <row r="28" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
-      <c r="B28" s="148"/>
-      <c r="C28" s="149"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="65"/>
       <c r="D28" s="8"/>
       <c r="G28" s="3"/>
       <c r="J28" s="12"/>
@@ -5424,8 +5427,8 @@
     </row>
     <row r="29" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
-      <c r="B29" s="148"/>
-      <c r="C29" s="149"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="65"/>
       <c r="D29" s="8"/>
       <c r="G29" s="3"/>
       <c r="J29" s="12"/>
@@ -5434,8 +5437,8 @@
     </row>
     <row r="30" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
-      <c r="B30" s="148"/>
-      <c r="C30" s="149"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="65"/>
       <c r="D30" s="8"/>
       <c r="G30" s="3"/>
       <c r="J30" s="12"/>
@@ -5444,8 +5447,8 @@
     </row>
     <row r="31" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
-      <c r="B31" s="148"/>
-      <c r="C31" s="149"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="65"/>
       <c r="D31" s="8"/>
       <c r="G31" s="3"/>
       <c r="J31" s="12"/>
@@ -5454,8 +5457,8 @@
     </row>
     <row r="32" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
-      <c r="B32" s="148"/>
-      <c r="C32" s="149"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="65"/>
       <c r="D32" s="8"/>
       <c r="G32" s="3"/>
       <c r="I32" s="32"/>
@@ -5465,8 +5468,8 @@
     </row>
     <row r="33" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
-      <c r="B33" s="148"/>
-      <c r="C33" s="149"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="65"/>
       <c r="D33" s="8"/>
       <c r="G33" s="3"/>
       <c r="J33" s="12"/>
@@ -5475,8 +5478,8 @@
     </row>
     <row r="34" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
-      <c r="B34" s="148"/>
-      <c r="C34" s="149"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="65"/>
       <c r="D34" s="8"/>
       <c r="G34" s="3"/>
       <c r="J34" s="12"/>
@@ -5485,8 +5488,8 @@
     </row>
     <row r="35" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
-      <c r="B35" s="148"/>
-      <c r="C35" s="149"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="65"/>
       <c r="D35" s="8"/>
       <c r="G35" s="3"/>
       <c r="J35" s="12"/>
@@ -5495,8 +5498,8 @@
     </row>
     <row r="36" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
-      <c r="B36" s="148"/>
-      <c r="C36" s="149"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="65"/>
       <c r="D36" s="8"/>
       <c r="G36" s="3"/>
       <c r="J36" s="12"/>
@@ -5504,8 +5507,8 @@
     </row>
     <row r="37" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
-      <c r="B37" s="148"/>
-      <c r="C37" s="149"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="65"/>
       <c r="D37" s="8"/>
       <c r="G37" s="3"/>
       <c r="J37" s="12"/>
@@ -5513,8 +5516,8 @@
     </row>
     <row r="38" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
-      <c r="B38" s="148"/>
-      <c r="C38" s="149"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="65"/>
       <c r="D38" s="8"/>
       <c r="G38" s="3"/>
       <c r="J38" s="12"/>
@@ -5522,8 +5525,8 @@
     </row>
     <row r="39" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
-      <c r="B39" s="148"/>
-      <c r="C39" s="149"/>
+      <c r="B39" s="64"/>
+      <c r="C39" s="65"/>
       <c r="D39" s="8"/>
       <c r="G39" s="3"/>
       <c r="J39" s="12"/>
@@ -5531,8 +5534,8 @@
     </row>
     <row r="40" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
-      <c r="B40" s="148"/>
-      <c r="C40" s="149"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="65"/>
       <c r="D40" s="8"/>
       <c r="G40" s="3"/>
       <c r="J40" s="12"/>
@@ -5540,8 +5543,8 @@
     </row>
     <row r="41" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
-      <c r="B41" s="148"/>
-      <c r="C41" s="149"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="65"/>
       <c r="D41" s="8"/>
       <c r="G41" s="3"/>
       <c r="J41" s="12"/>
@@ -5550,8 +5553,8 @@
     </row>
     <row r="42" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
-      <c r="B42" s="148"/>
-      <c r="C42" s="149"/>
+      <c r="B42" s="64"/>
+      <c r="C42" s="65"/>
       <c r="D42" s="8"/>
       <c r="G42" s="3"/>
       <c r="J42" s="12"/>
@@ -5559,8 +5562,8 @@
     </row>
     <row r="43" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
-      <c r="B43" s="148"/>
-      <c r="C43" s="149"/>
+      <c r="B43" s="64"/>
+      <c r="C43" s="65"/>
       <c r="D43" s="8"/>
       <c r="G43" s="3"/>
       <c r="J43" s="12"/>
@@ -5568,8 +5571,8 @@
     </row>
     <row r="44" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
-      <c r="B44" s="148"/>
-      <c r="C44" s="149"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="65"/>
       <c r="D44" s="8"/>
       <c r="G44" s="3"/>
       <c r="J44" s="12"/>
@@ -5577,8 +5580,8 @@
     </row>
     <row r="45" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
-      <c r="B45" s="148"/>
-      <c r="C45" s="149"/>
+      <c r="B45" s="64"/>
+      <c r="C45" s="65"/>
       <c r="D45" s="8"/>
       <c r="G45" s="3"/>
       <c r="J45" s="12"/>
@@ -5586,8 +5589,8 @@
     </row>
     <row r="46" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
-      <c r="B46" s="148"/>
-      <c r="C46" s="149"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="65"/>
       <c r="D46" s="8"/>
       <c r="G46" s="3"/>
       <c r="J46" s="12"/>
@@ -5596,8 +5599,8 @@
     </row>
     <row r="47" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
-      <c r="B47" s="148"/>
-      <c r="C47" s="149"/>
+      <c r="B47" s="64"/>
+      <c r="C47" s="65"/>
       <c r="D47" s="8"/>
       <c r="G47" s="3"/>
       <c r="J47" s="12"/>
@@ -5606,8 +5609,8 @@
     </row>
     <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
-      <c r="B48" s="148"/>
-      <c r="C48" s="149"/>
+      <c r="B48" s="64"/>
+      <c r="C48" s="65"/>
       <c r="D48" s="8"/>
       <c r="G48" s="3"/>
       <c r="J48" s="12"/>
@@ -5616,8 +5619,8 @@
     </row>
     <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
-      <c r="B49" s="148"/>
-      <c r="C49" s="149"/>
+      <c r="B49" s="64"/>
+      <c r="C49" s="65"/>
       <c r="D49" s="8"/>
       <c r="G49" s="3"/>
       <c r="J49" s="12"/>
@@ -5627,8 +5630,8 @@
     </row>
     <row r="50" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
-      <c r="B50" s="148"/>
-      <c r="C50" s="149"/>
+      <c r="B50" s="64"/>
+      <c r="C50" s="65"/>
       <c r="D50" s="8"/>
       <c r="G50" s="3"/>
       <c r="J50" s="12"/>
@@ -5637,8 +5640,8 @@
     </row>
     <row r="51" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
-      <c r="B51" s="148"/>
-      <c r="C51" s="149"/>
+      <c r="B51" s="64"/>
+      <c r="C51" s="65"/>
       <c r="D51" s="8"/>
       <c r="G51" s="3"/>
       <c r="J51" s="12"/>
@@ -5646,8 +5649,8 @@
     </row>
     <row r="52" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
-      <c r="B52" s="148"/>
-      <c r="C52" s="149"/>
+      <c r="B52" s="64"/>
+      <c r="C52" s="65"/>
       <c r="D52" s="8"/>
       <c r="G52" s="3"/>
       <c r="J52" s="12"/>
@@ -5655,8 +5658,8 @@
     </row>
     <row r="53" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
-      <c r="B53" s="148"/>
-      <c r="C53" s="149"/>
+      <c r="B53" s="64"/>
+      <c r="C53" s="65"/>
       <c r="D53" s="8"/>
       <c r="G53" s="3"/>
       <c r="J53" s="12"/>
@@ -5664,8 +5667,8 @@
     </row>
     <row r="54" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
-      <c r="B54" s="148"/>
-      <c r="C54" s="149"/>
+      <c r="B54" s="64"/>
+      <c r="C54" s="65"/>
       <c r="D54" s="8"/>
       <c r="G54" s="3"/>
       <c r="J54" s="12"/>
@@ -5674,8 +5677,8 @@
     </row>
     <row r="55" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
-      <c r="B55" s="148"/>
-      <c r="C55" s="149"/>
+      <c r="B55" s="64"/>
+      <c r="C55" s="65"/>
       <c r="D55" s="8"/>
       <c r="G55" s="3"/>
       <c r="J55" s="12"/>
@@ -5684,8 +5687,8 @@
     </row>
     <row r="56" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
-      <c r="B56" s="148"/>
-      <c r="C56" s="149"/>
+      <c r="B56" s="64"/>
+      <c r="C56" s="65"/>
       <c r="D56" s="8"/>
       <c r="G56" s="3"/>
       <c r="J56" s="12"/>
@@ -5694,8 +5697,8 @@
     </row>
     <row r="57" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
-      <c r="B57" s="148"/>
-      <c r="C57" s="149"/>
+      <c r="B57" s="64"/>
+      <c r="C57" s="65"/>
       <c r="D57" s="8"/>
       <c r="G57" s="3"/>
       <c r="J57" s="12"/>
@@ -5704,8 +5707,8 @@
     </row>
     <row r="58" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
-      <c r="B58" s="148"/>
-      <c r="C58" s="149"/>
+      <c r="B58" s="64"/>
+      <c r="C58" s="65"/>
       <c r="D58" s="8"/>
       <c r="G58" s="3"/>
       <c r="J58" s="12"/>
@@ -5713,8 +5716,8 @@
     </row>
     <row r="59" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
-      <c r="B59" s="148"/>
-      <c r="C59" s="149"/>
+      <c r="B59" s="64"/>
+      <c r="C59" s="65"/>
       <c r="D59" s="8"/>
       <c r="G59" s="3"/>
       <c r="J59" s="12"/>
@@ -5722,8 +5725,8 @@
     </row>
     <row r="60" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
-      <c r="B60" s="148"/>
-      <c r="C60" s="149"/>
+      <c r="B60" s="64"/>
+      <c r="C60" s="65"/>
       <c r="D60" s="8"/>
       <c r="G60" s="3"/>
       <c r="J60" s="12"/>
@@ -5731,8 +5734,8 @@
     </row>
     <row r="61" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
-      <c r="B61" s="148"/>
-      <c r="C61" s="149"/>
+      <c r="B61" s="64"/>
+      <c r="C61" s="65"/>
       <c r="D61" s="8"/>
       <c r="G61" s="3"/>
       <c r="J61" s="12"/>
@@ -5740,8 +5743,8 @@
     </row>
     <row r="62" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
-      <c r="B62" s="148"/>
-      <c r="C62" s="149"/>
+      <c r="B62" s="64"/>
+      <c r="C62" s="65"/>
       <c r="D62" s="8"/>
       <c r="G62" s="3"/>
       <c r="J62" s="12"/>
@@ -5749,8 +5752,8 @@
     </row>
     <row r="63" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
-      <c r="B63" s="148"/>
-      <c r="C63" s="149"/>
+      <c r="B63" s="64"/>
+      <c r="C63" s="65"/>
       <c r="D63" s="8"/>
       <c r="G63" s="3"/>
       <c r="J63" s="12"/>
@@ -5759,8 +5762,8 @@
     </row>
     <row r="64" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
-      <c r="B64" s="148"/>
-      <c r="C64" s="149"/>
+      <c r="B64" s="64"/>
+      <c r="C64" s="65"/>
       <c r="D64" s="8"/>
       <c r="G64" s="3"/>
       <c r="J64" s="12"/>
@@ -5768,8 +5771,8 @@
     </row>
     <row r="65" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
-      <c r="B65" s="148"/>
-      <c r="C65" s="149"/>
+      <c r="B65" s="64"/>
+      <c r="C65" s="65"/>
       <c r="D65" s="8"/>
       <c r="G65" s="3"/>
       <c r="J65" s="12"/>
@@ -5778,8 +5781,8 @@
     </row>
     <row r="66" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
-      <c r="B66" s="148"/>
-      <c r="C66" s="149"/>
+      <c r="B66" s="64"/>
+      <c r="C66" s="65"/>
       <c r="D66" s="8"/>
       <c r="G66" s="3"/>
       <c r="J66" s="12"/>
@@ -5787,8 +5790,8 @@
     </row>
     <row r="67" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
-      <c r="B67" s="148"/>
-      <c r="C67" s="149"/>
+      <c r="B67" s="64"/>
+      <c r="C67" s="65"/>
       <c r="D67" s="8"/>
       <c r="G67" s="3"/>
       <c r="J67" s="12"/>
@@ -5796,8 +5799,8 @@
     </row>
     <row r="68" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
-      <c r="B68" s="148"/>
-      <c r="C68" s="149"/>
+      <c r="B68" s="64"/>
+      <c r="C68" s="65"/>
       <c r="D68" s="8"/>
       <c r="G68" s="3"/>
       <c r="J68" s="12"/>
@@ -5805,8 +5808,8 @@
     </row>
     <row r="69" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
-      <c r="B69" s="148"/>
-      <c r="C69" s="149"/>
+      <c r="B69" s="64"/>
+      <c r="C69" s="65"/>
       <c r="D69" s="8"/>
       <c r="G69" s="3"/>
       <c r="J69" s="12"/>
@@ -5814,8 +5817,8 @@
     </row>
     <row r="70" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
-      <c r="B70" s="148"/>
-      <c r="C70" s="148"/>
+      <c r="B70" s="64"/>
+      <c r="C70" s="64"/>
       <c r="D70" s="8"/>
       <c r="G70" s="3"/>
       <c r="J70" s="12"/>
@@ -5823,8 +5826,8 @@
     </row>
     <row r="71" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
-      <c r="B71" s="148"/>
-      <c r="C71" s="148"/>
+      <c r="B71" s="64"/>
+      <c r="C71" s="64"/>
       <c r="D71" s="8"/>
       <c r="G71" s="3"/>
       <c r="J71" s="12"/>
@@ -5832,8 +5835,8 @@
     </row>
     <row r="72" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
-      <c r="B72" s="148"/>
-      <c r="C72" s="148"/>
+      <c r="B72" s="64"/>
+      <c r="C72" s="64"/>
       <c r="D72" s="8"/>
       <c r="G72" s="3"/>
       <c r="J72" s="12"/>
@@ -5841,8 +5844,8 @@
     </row>
     <row r="73" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
-      <c r="B73" s="148"/>
-      <c r="C73" s="148"/>
+      <c r="B73" s="64"/>
+      <c r="C73" s="64"/>
       <c r="D73" s="8"/>
       <c r="G73" s="3"/>
       <c r="J73" s="12"/>
@@ -5850,8 +5853,8 @@
     </row>
     <row r="74" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="3"/>
-      <c r="B74" s="148"/>
-      <c r="C74" s="148"/>
+      <c r="B74" s="64"/>
+      <c r="C74" s="64"/>
       <c r="D74" s="8"/>
       <c r="G74" s="3"/>
       <c r="J74" s="12"/>
@@ -5860,8 +5863,8 @@
     </row>
     <row r="75" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
-      <c r="B75" s="148"/>
-      <c r="C75" s="148"/>
+      <c r="B75" s="64"/>
+      <c r="C75" s="64"/>
       <c r="D75" s="8"/>
       <c r="G75" s="3"/>
       <c r="J75" s="12"/>
@@ -5869,8 +5872,8 @@
     </row>
     <row r="76" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3"/>
-      <c r="B76" s="148"/>
-      <c r="C76" s="148"/>
+      <c r="B76" s="64"/>
+      <c r="C76" s="64"/>
       <c r="D76" s="8"/>
       <c r="G76" s="3"/>
       <c r="J76" s="12"/>
@@ -5878,8 +5881,8 @@
     </row>
     <row r="77" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="3"/>
-      <c r="B77" s="148"/>
-      <c r="C77" s="148"/>
+      <c r="B77" s="64"/>
+      <c r="C77" s="64"/>
       <c r="D77" s="8"/>
       <c r="G77" s="3"/>
       <c r="J77" s="12"/>
@@ -5888,8 +5891,8 @@
     </row>
     <row r="78" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3"/>
-      <c r="B78" s="148"/>
-      <c r="C78" s="148"/>
+      <c r="B78" s="64"/>
+      <c r="C78" s="64"/>
       <c r="D78" s="8"/>
       <c r="G78" s="3"/>
       <c r="J78" s="12"/>
@@ -5897,8 +5900,8 @@
     </row>
     <row r="79" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3"/>
-      <c r="B79" s="148"/>
-      <c r="C79" s="148"/>
+      <c r="B79" s="64"/>
+      <c r="C79" s="64"/>
       <c r="D79" s="8"/>
       <c r="G79" s="3"/>
       <c r="J79" s="12"/>
@@ -5906,8 +5909,8 @@
     </row>
     <row r="80" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
-      <c r="B80" s="148"/>
-      <c r="C80" s="148"/>
+      <c r="B80" s="64"/>
+      <c r="C80" s="64"/>
       <c r="D80" s="8"/>
       <c r="G80" s="3"/>
       <c r="J80" s="12"/>
@@ -5915,8 +5918,8 @@
     </row>
     <row r="81" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
-      <c r="B81" s="148"/>
-      <c r="C81" s="148"/>
+      <c r="B81" s="64"/>
+      <c r="C81" s="64"/>
       <c r="D81" s="8"/>
       <c r="G81" s="3"/>
       <c r="J81" s="12"/>
@@ -5924,8 +5927,8 @@
     </row>
     <row r="82" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3"/>
-      <c r="B82" s="148"/>
-      <c r="C82" s="148"/>
+      <c r="B82" s="64"/>
+      <c r="C82" s="64"/>
       <c r="D82" s="8"/>
       <c r="E82" s="36"/>
       <c r="F82" s="36"/>
@@ -5937,8 +5940,8 @@
     </row>
     <row r="83" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3"/>
-      <c r="B83" s="148"/>
-      <c r="C83" s="148"/>
+      <c r="B83" s="64"/>
+      <c r="C83" s="64"/>
       <c r="D83" s="8"/>
       <c r="G83" s="3"/>
       <c r="J83" s="12"/>
@@ -5946,8 +5949,8 @@
     </row>
     <row r="84" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="3"/>
-      <c r="B84" s="148"/>
-      <c r="C84" s="148"/>
+      <c r="B84" s="64"/>
+      <c r="C84" s="64"/>
       <c r="D84" s="8"/>
       <c r="G84" s="3"/>
       <c r="J84" s="12"/>
@@ -5956,8 +5959,8 @@
     </row>
     <row r="85" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3"/>
-      <c r="B85" s="148"/>
-      <c r="C85" s="148"/>
+      <c r="B85" s="64"/>
+      <c r="C85" s="64"/>
       <c r="D85" s="8"/>
       <c r="G85" s="3"/>
       <c r="J85" s="12"/>
@@ -5965,8 +5968,8 @@
     </row>
     <row r="86" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3"/>
-      <c r="B86" s="148"/>
-      <c r="C86" s="148"/>
+      <c r="B86" s="64"/>
+      <c r="C86" s="64"/>
       <c r="D86" s="8"/>
       <c r="G86" s="3"/>
       <c r="J86" s="12"/>
@@ -5974,8 +5977,8 @@
     </row>
     <row r="87" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3"/>
-      <c r="B87" s="148"/>
-      <c r="C87" s="148"/>
+      <c r="B87" s="64"/>
+      <c r="C87" s="64"/>
       <c r="D87" s="8"/>
       <c r="G87" s="3"/>
       <c r="J87" s="12"/>
@@ -5983,8 +5986,8 @@
     </row>
     <row r="88" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A88" s="3"/>
-      <c r="B88" s="148"/>
-      <c r="C88" s="148"/>
+      <c r="B88" s="64"/>
+      <c r="C88" s="64"/>
       <c r="D88" s="8"/>
       <c r="G88" s="3"/>
       <c r="J88" s="12"/>
@@ -5993,8 +5996,8 @@
     </row>
     <row r="89" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
-      <c r="B89" s="148"/>
-      <c r="C89" s="148"/>
+      <c r="B89" s="64"/>
+      <c r="C89" s="64"/>
       <c r="D89" s="8"/>
       <c r="G89" s="3"/>
       <c r="J89" s="12"/>
@@ -6003,8 +6006,8 @@
     </row>
     <row r="90" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A90" s="3"/>
-      <c r="B90" s="148"/>
-      <c r="C90" s="148"/>
+      <c r="B90" s="64"/>
+      <c r="C90" s="64"/>
       <c r="D90" s="8"/>
       <c r="G90" s="3"/>
       <c r="J90" s="12"/>
@@ -6013,8 +6016,8 @@
     </row>
     <row r="91" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A91" s="3"/>
-      <c r="B91" s="148"/>
-      <c r="C91" s="148"/>
+      <c r="B91" s="64"/>
+      <c r="C91" s="64"/>
       <c r="D91" s="8"/>
       <c r="G91" s="3"/>
       <c r="J91" s="12"/>
@@ -6023,8 +6026,8 @@
     </row>
     <row r="92" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A92" s="3"/>
-      <c r="B92" s="148"/>
-      <c r="C92" s="148"/>
+      <c r="B92" s="64"/>
+      <c r="C92" s="64"/>
       <c r="D92" s="8"/>
       <c r="G92" s="3"/>
       <c r="J92" s="12"/>
@@ -6033,8 +6036,8 @@
     </row>
     <row r="93" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3"/>
-      <c r="B93" s="148"/>
-      <c r="C93" s="148"/>
+      <c r="B93" s="64"/>
+      <c r="C93" s="64"/>
       <c r="D93" s="8"/>
       <c r="G93" s="3"/>
       <c r="J93" s="12"/>
@@ -6042,8 +6045,8 @@
     </row>
     <row r="94" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3"/>
-      <c r="B94" s="148"/>
-      <c r="C94" s="148"/>
+      <c r="B94" s="64"/>
+      <c r="C94" s="64"/>
       <c r="D94" s="8"/>
       <c r="G94" s="3"/>
       <c r="J94" s="12"/>
@@ -6051,8 +6054,8 @@
     </row>
     <row r="95" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="3"/>
-      <c r="B95" s="148"/>
-      <c r="C95" s="148"/>
+      <c r="B95" s="64"/>
+      <c r="C95" s="64"/>
       <c r="D95" s="8"/>
       <c r="G95" s="3"/>
       <c r="J95" s="12"/>
@@ -6061,8 +6064,8 @@
     </row>
     <row r="96" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3"/>
-      <c r="B96" s="148"/>
-      <c r="C96" s="148"/>
+      <c r="B96" s="64"/>
+      <c r="C96" s="64"/>
       <c r="D96" s="8"/>
       <c r="G96" s="3"/>
       <c r="J96" s="12"/>
@@ -6070,8 +6073,8 @@
     </row>
     <row r="97" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3"/>
-      <c r="B97" s="148"/>
-      <c r="C97" s="148"/>
+      <c r="B97" s="64"/>
+      <c r="C97" s="64"/>
       <c r="D97" s="8"/>
       <c r="G97" s="3"/>
       <c r="J97" s="12"/>
@@ -6079,8 +6082,8 @@
     </row>
     <row r="98" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3"/>
-      <c r="B98" s="148"/>
-      <c r="C98" s="148"/>
+      <c r="B98" s="64"/>
+      <c r="C98" s="64"/>
       <c r="D98" s="8"/>
       <c r="G98" s="3"/>
       <c r="J98" s="12"/>
@@ -6088,24 +6091,24 @@
     </row>
     <row r="99" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3"/>
-      <c r="B99" s="148"/>
-      <c r="C99" s="148"/>
+      <c r="B99" s="64"/>
+      <c r="C99" s="64"/>
       <c r="G99" s="3"/>
       <c r="J99" s="12"/>
       <c r="N99" s="35"/>
     </row>
     <row r="100" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3"/>
-      <c r="B100" s="148"/>
-      <c r="C100" s="148"/>
+      <c r="B100" s="64"/>
+      <c r="C100" s="64"/>
       <c r="G100" s="3"/>
       <c r="J100" s="12"/>
       <c r="N100" s="35"/>
     </row>
     <row r="101" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3"/>
-      <c r="B101" s="148"/>
-      <c r="C101" s="148"/>
+      <c r="B101" s="64"/>
+      <c r="C101" s="64"/>
       <c r="F101" s="43"/>
       <c r="G101" s="3"/>
       <c r="H101" s="42"/>
@@ -6114,16 +6117,16 @@
     </row>
     <row r="102" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3"/>
-      <c r="B102" s="148"/>
-      <c r="C102" s="148"/>
+      <c r="B102" s="64"/>
+      <c r="C102" s="64"/>
       <c r="G102" s="3"/>
       <c r="J102" s="12"/>
       <c r="N102" s="35"/>
     </row>
     <row r="103" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="3"/>
-      <c r="B103" s="148"/>
-      <c r="C103" s="148"/>
+      <c r="B103" s="64"/>
+      <c r="C103" s="64"/>
       <c r="G103" s="3"/>
       <c r="J103" s="12"/>
       <c r="L103" s="38"/>
@@ -6131,48 +6134,48 @@
     </row>
     <row r="104" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3"/>
-      <c r="B104" s="148"/>
-      <c r="C104" s="148"/>
+      <c r="B104" s="64"/>
+      <c r="C104" s="64"/>
       <c r="G104" s="3"/>
       <c r="J104" s="12"/>
       <c r="N104" s="35"/>
     </row>
     <row r="105" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3"/>
-      <c r="B105" s="148"/>
-      <c r="C105" s="148"/>
+      <c r="B105" s="64"/>
+      <c r="C105" s="64"/>
       <c r="G105" s="3"/>
       <c r="J105" s="12"/>
       <c r="N105" s="35"/>
     </row>
     <row r="106" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3"/>
-      <c r="B106" s="148"/>
-      <c r="C106" s="148"/>
+      <c r="B106" s="64"/>
+      <c r="C106" s="64"/>
       <c r="G106" s="3"/>
       <c r="J106" s="12"/>
       <c r="N106" s="35"/>
     </row>
     <row r="107" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3"/>
-      <c r="B107" s="148"/>
-      <c r="C107" s="148"/>
+      <c r="B107" s="64"/>
+      <c r="C107" s="64"/>
       <c r="G107" s="3"/>
       <c r="J107" s="12"/>
       <c r="N107" s="35"/>
     </row>
     <row r="108" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3"/>
-      <c r="B108" s="148"/>
-      <c r="C108" s="148"/>
+      <c r="B108" s="64"/>
+      <c r="C108" s="64"/>
       <c r="G108" s="3"/>
       <c r="J108" s="12"/>
       <c r="N108" s="35"/>
     </row>
     <row r="109" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="3"/>
-      <c r="B109" s="148"/>
-      <c r="C109" s="148"/>
+      <c r="B109" s="64"/>
+      <c r="C109" s="64"/>
       <c r="G109" s="3"/>
       <c r="J109" s="12"/>
       <c r="L109" s="38"/>
@@ -6180,48 +6183,48 @@
     </row>
     <row r="110" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3"/>
-      <c r="B110" s="148"/>
-      <c r="C110" s="148"/>
+      <c r="B110" s="64"/>
+      <c r="C110" s="64"/>
       <c r="G110" s="3"/>
       <c r="J110" s="12"/>
       <c r="N110" s="35"/>
     </row>
     <row r="111" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3"/>
-      <c r="B111" s="148"/>
-      <c r="C111" s="148"/>
+      <c r="B111" s="64"/>
+      <c r="C111" s="64"/>
       <c r="G111" s="3"/>
       <c r="J111" s="12"/>
       <c r="N111" s="35"/>
     </row>
     <row r="112" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3"/>
-      <c r="B112" s="148"/>
-      <c r="C112" s="148"/>
+      <c r="B112" s="64"/>
+      <c r="C112" s="64"/>
       <c r="G112" s="3"/>
       <c r="J112" s="12"/>
       <c r="N112" s="35"/>
     </row>
     <row r="113" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3"/>
-      <c r="B113" s="148"/>
-      <c r="C113" s="148"/>
+      <c r="B113" s="64"/>
+      <c r="C113" s="64"/>
       <c r="G113" s="3"/>
       <c r="J113" s="12"/>
       <c r="N113" s="35"/>
     </row>
     <row r="114" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3"/>
-      <c r="B114" s="148"/>
-      <c r="C114" s="148"/>
+      <c r="B114" s="64"/>
+      <c r="C114" s="64"/>
       <c r="G114" s="3"/>
       <c r="J114" s="12"/>
       <c r="N114" s="35"/>
     </row>
     <row r="115" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A115" s="3"/>
-      <c r="B115" s="148"/>
-      <c r="C115" s="148"/>
+      <c r="B115" s="64"/>
+      <c r="C115" s="64"/>
       <c r="G115" s="3"/>
       <c r="J115" s="12"/>
       <c r="L115" s="38"/>
@@ -6229,16 +6232,16 @@
     </row>
     <row r="116" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3"/>
-      <c r="B116" s="148"/>
-      <c r="C116" s="148"/>
+      <c r="B116" s="64"/>
+      <c r="C116" s="64"/>
       <c r="G116" s="3"/>
       <c r="J116" s="12"/>
       <c r="N116" s="35"/>
     </row>
     <row r="117" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A117" s="3"/>
-      <c r="B117" s="148"/>
-      <c r="C117" s="148"/>
+      <c r="B117" s="64"/>
+      <c r="C117" s="64"/>
       <c r="G117" s="3"/>
       <c r="J117" s="12"/>
       <c r="L117" s="38"/>
@@ -6246,24 +6249,24 @@
     </row>
     <row r="118" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3"/>
-      <c r="B118" s="148"/>
-      <c r="C118" s="148"/>
+      <c r="B118" s="64"/>
+      <c r="C118" s="64"/>
       <c r="G118" s="3"/>
       <c r="J118" s="12"/>
       <c r="N118" s="35"/>
     </row>
     <row r="119" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3"/>
-      <c r="B119" s="148"/>
-      <c r="C119" s="148"/>
+      <c r="B119" s="64"/>
+      <c r="C119" s="64"/>
       <c r="G119" s="3"/>
       <c r="J119" s="12"/>
       <c r="N119" s="35"/>
     </row>
     <row r="120" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A120" s="3"/>
-      <c r="B120" s="148"/>
-      <c r="C120" s="148"/>
+      <c r="B120" s="64"/>
+      <c r="C120" s="64"/>
       <c r="G120" s="3"/>
       <c r="J120" s="12"/>
       <c r="K120" s="38"/>
@@ -6271,22 +6274,22 @@
     </row>
     <row r="121" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3"/>
-      <c r="B121" s="148"/>
-      <c r="C121" s="148"/>
+      <c r="B121" s="64"/>
+      <c r="C121" s="64"/>
       <c r="G121" s="3"/>
       <c r="N121" s="35"/>
     </row>
     <row r="122" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3"/>
-      <c r="B122" s="148"/>
-      <c r="C122" s="148"/>
+      <c r="B122" s="64"/>
+      <c r="C122" s="64"/>
       <c r="G122" s="3"/>
       <c r="N122" s="35"/>
     </row>
     <row r="123" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3"/>
-      <c r="B123" s="148"/>
-      <c r="C123" s="148"/>
+      <c r="B123" s="64"/>
+      <c r="C123" s="64"/>
       <c r="G123" s="3"/>
       <c r="N123" s="35"/>
     </row>
@@ -6331,6 +6334,14 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="B10:B24"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C10:C16"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
@@ -6338,14 +6349,6 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C10:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C20:C24"/>
-    <mergeCell ref="B10:B24"/>
   </mergeCells>
   <conditionalFormatting sqref="N10:N24 N125:N136">
     <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
@@ -6423,106 +6426,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="108" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="121"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="111"/>
     </row>
     <row r="2" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="134" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="134"/>
-      <c r="E2" s="135"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="124" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="124"/>
+      <c r="E2" s="125"/>
     </row>
     <row r="3" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="129" t="s">
+      <c r="A3" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="130"/>
-      <c r="C3" s="124" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="125"/>
-      <c r="E3" s="126"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="114" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="115"/>
+      <c r="E3" s="116"/>
     </row>
     <row r="4" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="129" t="s">
+      <c r="A4" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="130"/>
-      <c r="C4" s="124">
+      <c r="B4" s="120"/>
+      <c r="C4" s="114">
         <v>4</v>
       </c>
-      <c r="D4" s="125"/>
-      <c r="E4" s="126"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="116"/>
     </row>
     <row r="5" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="129" t="s">
+      <c r="A5" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="130"/>
-      <c r="C5" s="124">
+      <c r="B5" s="120"/>
+      <c r="C5" s="114">
         <v>1</v>
       </c>
-      <c r="D5" s="125"/>
-      <c r="E5" s="126"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="116"/>
     </row>
     <row r="6" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="129" t="s">
+      <c r="A6" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="130"/>
-      <c r="C6" s="124" t="s">
+      <c r="B6" s="120"/>
+      <c r="C6" s="114" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="125"/>
-      <c r="E6" s="126"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="116"/>
     </row>
     <row r="7" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="129" t="s">
+      <c r="A7" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="130"/>
-      <c r="C7" s="124" t="s">
+      <c r="B7" s="120"/>
+      <c r="C7" s="114" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="125"/>
-      <c r="E7" s="126"/>
+      <c r="D7" s="115"/>
+      <c r="E7" s="116"/>
     </row>
     <row r="8" spans="1:14" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="122" t="s">
+      <c r="A8" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="123"/>
-      <c r="C8" s="131"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="133"/>
+      <c r="B8" s="113"/>
+      <c r="C8" s="121"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="123"/>
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="100" t="s">
+      <c r="B10" s="155" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="J10" s="79" t="s">
+      <c r="C10" s="156"/>
+      <c r="D10" s="156"/>
+      <c r="E10" s="156"/>
+      <c r="F10" s="156"/>
+      <c r="G10" s="157"/>
+      <c r="J10" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="K10" s="80"/>
-      <c r="L10" s="80"/>
-      <c r="M10" s="80"/>
-      <c r="N10" s="81"/>
+      <c r="K10" s="135"/>
+      <c r="L10" s="135"/>
+      <c r="M10" s="135"/>
+      <c r="N10" s="136"/>
     </row>
     <row r="11" spans="1:14" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
@@ -6678,185 +6681,185 @@
       <c r="G31" s="16"/>
     </row>
     <row r="32" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="82"/>
-      <c r="C32" s="85" t="s">
+      <c r="B32" s="137"/>
+      <c r="C32" s="140" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="86"/>
-      <c r="E32" s="91" t="s">
+      <c r="D32" s="141"/>
+      <c r="E32" s="146" t="s">
         <v>53</v>
       </c>
-      <c r="F32" s="92"/>
-      <c r="G32" s="92"/>
-      <c r="H32" s="93"/>
+      <c r="F32" s="147"/>
+      <c r="G32" s="147"/>
+      <c r="H32" s="148"/>
     </row>
     <row r="33" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="83"/>
-      <c r="C33" s="87"/>
-      <c r="D33" s="88"/>
-      <c r="E33" s="94"/>
-      <c r="F33" s="95"/>
-      <c r="G33" s="95"/>
-      <c r="H33" s="96"/>
+      <c r="B33" s="138"/>
+      <c r="C33" s="142"/>
+      <c r="D33" s="143"/>
+      <c r="E33" s="149"/>
+      <c r="F33" s="150"/>
+      <c r="G33" s="150"/>
+      <c r="H33" s="151"/>
     </row>
     <row r="34" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="83"/>
-      <c r="C34" s="87"/>
-      <c r="D34" s="88"/>
-      <c r="E34" s="94"/>
-      <c r="F34" s="95"/>
-      <c r="G34" s="95"/>
-      <c r="H34" s="96"/>
+      <c r="B34" s="138"/>
+      <c r="C34" s="142"/>
+      <c r="D34" s="143"/>
+      <c r="E34" s="149"/>
+      <c r="F34" s="150"/>
+      <c r="G34" s="150"/>
+      <c r="H34" s="151"/>
     </row>
     <row r="35" spans="2:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="84"/>
-      <c r="C35" s="89"/>
-      <c r="D35" s="90"/>
-      <c r="E35" s="97"/>
-      <c r="F35" s="98"/>
-      <c r="G35" s="98"/>
-      <c r="H35" s="99"/>
+      <c r="B35" s="139"/>
+      <c r="C35" s="144"/>
+      <c r="D35" s="145"/>
+      <c r="E35" s="152"/>
+      <c r="F35" s="153"/>
+      <c r="G35" s="153"/>
+      <c r="H35" s="154"/>
     </row>
     <row r="36" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="115" t="s">
+      <c r="B36" s="133" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="103" t="s">
+      <c r="C36" s="126" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="104"/>
-      <c r="E36" s="107" t="s">
+      <c r="D36" s="127"/>
+      <c r="E36" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="F36" s="108"/>
-      <c r="G36" s="108"/>
-      <c r="H36" s="109"/>
+      <c r="F36" s="131"/>
+      <c r="G36" s="131"/>
+      <c r="H36" s="132"/>
     </row>
     <row r="37" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="114"/>
-      <c r="C37" s="105"/>
-      <c r="D37" s="106"/>
-      <c r="E37" s="110"/>
-      <c r="F37" s="111"/>
-      <c r="G37" s="111"/>
-      <c r="H37" s="112"/>
+      <c r="B37" s="90"/>
+      <c r="C37" s="128"/>
+      <c r="D37" s="129"/>
+      <c r="E37" s="94"/>
+      <c r="F37" s="95"/>
+      <c r="G37" s="95"/>
+      <c r="H37" s="96"/>
     </row>
     <row r="38" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="114"/>
-      <c r="C38" s="105"/>
-      <c r="D38" s="106"/>
-      <c r="E38" s="110"/>
-      <c r="F38" s="111"/>
-      <c r="G38" s="111"/>
-      <c r="H38" s="112"/>
+      <c r="B38" s="90"/>
+      <c r="C38" s="128"/>
+      <c r="D38" s="129"/>
+      <c r="E38" s="94"/>
+      <c r="F38" s="95"/>
+      <c r="G38" s="95"/>
+      <c r="H38" s="96"/>
     </row>
     <row r="39" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="114"/>
-      <c r="C39" s="105"/>
-      <c r="D39" s="106"/>
-      <c r="E39" s="110"/>
-      <c r="F39" s="111"/>
-      <c r="G39" s="111"/>
-      <c r="H39" s="112"/>
+      <c r="B39" s="90"/>
+      <c r="C39" s="128"/>
+      <c r="D39" s="129"/>
+      <c r="E39" s="94"/>
+      <c r="F39" s="95"/>
+      <c r="G39" s="95"/>
+      <c r="H39" s="96"/>
     </row>
     <row r="40" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="113" t="s">
+      <c r="B40" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="105" t="s">
+      <c r="C40" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="106"/>
-      <c r="E40" s="110" t="s">
+      <c r="D40" s="129"/>
+      <c r="E40" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="F40" s="111"/>
-      <c r="G40" s="111"/>
-      <c r="H40" s="112"/>
+      <c r="F40" s="95"/>
+      <c r="G40" s="95"/>
+      <c r="H40" s="96"/>
     </row>
     <row r="41" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="114"/>
-      <c r="C41" s="105"/>
-      <c r="D41" s="106"/>
-      <c r="E41" s="110"/>
-      <c r="F41" s="111"/>
-      <c r="G41" s="111"/>
-      <c r="H41" s="112"/>
+      <c r="B41" s="90"/>
+      <c r="C41" s="128"/>
+      <c r="D41" s="129"/>
+      <c r="E41" s="94"/>
+      <c r="F41" s="95"/>
+      <c r="G41" s="95"/>
+      <c r="H41" s="96"/>
     </row>
     <row r="42" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="114"/>
-      <c r="C42" s="105"/>
-      <c r="D42" s="106"/>
-      <c r="E42" s="110"/>
-      <c r="F42" s="111"/>
-      <c r="G42" s="111"/>
-      <c r="H42" s="112"/>
+      <c r="B42" s="90"/>
+      <c r="C42" s="128"/>
+      <c r="D42" s="129"/>
+      <c r="E42" s="94"/>
+      <c r="F42" s="95"/>
+      <c r="G42" s="95"/>
+      <c r="H42" s="96"/>
     </row>
     <row r="43" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="114"/>
-      <c r="C43" s="105"/>
-      <c r="D43" s="106"/>
-      <c r="E43" s="110"/>
-      <c r="F43" s="111"/>
-      <c r="G43" s="111"/>
-      <c r="H43" s="112"/>
+      <c r="B43" s="90"/>
+      <c r="C43" s="128"/>
+      <c r="D43" s="129"/>
+      <c r="E43" s="94"/>
+      <c r="F43" s="95"/>
+      <c r="G43" s="95"/>
+      <c r="H43" s="96"/>
     </row>
     <row r="44" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="113" t="s">
+      <c r="B44" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="105" t="s">
+      <c r="C44" s="128" t="s">
         <v>58</v>
       </c>
-      <c r="D44" s="106"/>
-      <c r="E44" s="110" t="s">
+      <c r="D44" s="129"/>
+      <c r="E44" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="F44" s="111"/>
-      <c r="G44" s="111"/>
-      <c r="H44" s="112"/>
+      <c r="F44" s="95"/>
+      <c r="G44" s="95"/>
+      <c r="H44" s="96"/>
     </row>
     <row r="45" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="114"/>
-      <c r="C45" s="105"/>
-      <c r="D45" s="106"/>
-      <c r="E45" s="110"/>
-      <c r="F45" s="111"/>
-      <c r="G45" s="111"/>
-      <c r="H45" s="112"/>
+      <c r="B45" s="90"/>
+      <c r="C45" s="128"/>
+      <c r="D45" s="129"/>
+      <c r="E45" s="94"/>
+      <c r="F45" s="95"/>
+      <c r="G45" s="95"/>
+      <c r="H45" s="96"/>
     </row>
     <row r="46" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="114"/>
-      <c r="C46" s="105"/>
-      <c r="D46" s="106"/>
-      <c r="E46" s="110"/>
-      <c r="F46" s="111"/>
-      <c r="G46" s="111"/>
-      <c r="H46" s="112"/>
+      <c r="B46" s="90"/>
+      <c r="C46" s="128"/>
+      <c r="D46" s="129"/>
+      <c r="E46" s="94"/>
+      <c r="F46" s="95"/>
+      <c r="G46" s="95"/>
+      <c r="H46" s="96"/>
     </row>
     <row r="47" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="114"/>
-      <c r="C47" s="105"/>
-      <c r="D47" s="106"/>
-      <c r="E47" s="110"/>
-      <c r="F47" s="111"/>
-      <c r="G47" s="111"/>
-      <c r="H47" s="112"/>
+      <c r="B47" s="90"/>
+      <c r="C47" s="128"/>
+      <c r="D47" s="129"/>
+      <c r="E47" s="94"/>
+      <c r="F47" s="95"/>
+      <c r="G47" s="95"/>
+      <c r="H47" s="96"/>
     </row>
     <row r="48" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="113" t="s">
+      <c r="B48" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="C48" s="105" t="s">
+      <c r="C48" s="128" t="s">
         <v>60</v>
       </c>
-      <c r="D48" s="106"/>
-      <c r="E48" s="110" t="s">
+      <c r="D48" s="129"/>
+      <c r="E48" s="94" t="s">
         <v>61</v>
       </c>
-      <c r="F48" s="111"/>
-      <c r="G48" s="111"/>
-      <c r="H48" s="112"/>
+      <c r="F48" s="95"/>
+      <c r="G48" s="95"/>
+      <c r="H48" s="96"/>
       <c r="L48" s="20"/>
       <c r="M48" s="17"/>
       <c r="N48" s="19"/>
@@ -6865,13 +6868,13 @@
       <c r="Q48" s="16"/>
     </row>
     <row r="49" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="114"/>
-      <c r="C49" s="105"/>
-      <c r="D49" s="106"/>
-      <c r="E49" s="110"/>
-      <c r="F49" s="111"/>
-      <c r="G49" s="111"/>
-      <c r="H49" s="112"/>
+      <c r="B49" s="90"/>
+      <c r="C49" s="128"/>
+      <c r="D49" s="129"/>
+      <c r="E49" s="94"/>
+      <c r="F49" s="95"/>
+      <c r="G49" s="95"/>
+      <c r="H49" s="96"/>
       <c r="L49" s="16"/>
       <c r="M49" s="16"/>
       <c r="N49" s="16"/>
@@ -6880,13 +6883,13 @@
       <c r="Q49" s="16"/>
     </row>
     <row r="50" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="114"/>
-      <c r="C50" s="105"/>
-      <c r="D50" s="106"/>
-      <c r="E50" s="110"/>
-      <c r="F50" s="111"/>
-      <c r="G50" s="111"/>
-      <c r="H50" s="112"/>
+      <c r="B50" s="90"/>
+      <c r="C50" s="128"/>
+      <c r="D50" s="129"/>
+      <c r="E50" s="94"/>
+      <c r="F50" s="95"/>
+      <c r="G50" s="95"/>
+      <c r="H50" s="96"/>
       <c r="L50" s="16"/>
       <c r="M50" s="16"/>
       <c r="N50" s="16"/>
@@ -6895,13 +6898,13 @@
       <c r="Q50" s="16"/>
     </row>
     <row r="51" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="114"/>
-      <c r="C51" s="105"/>
-      <c r="D51" s="106"/>
-      <c r="E51" s="110"/>
-      <c r="F51" s="111"/>
-      <c r="G51" s="111"/>
-      <c r="H51" s="112"/>
+      <c r="B51" s="90"/>
+      <c r="C51" s="128"/>
+      <c r="D51" s="129"/>
+      <c r="E51" s="94"/>
+      <c r="F51" s="95"/>
+      <c r="G51" s="95"/>
+      <c r="H51" s="96"/>
       <c r="L51" s="16"/>
       <c r="M51" s="16"/>
       <c r="N51" s="16"/>
@@ -6910,19 +6913,19 @@
       <c r="Q51" s="16"/>
     </row>
     <row r="52" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="113" t="s">
+      <c r="B52" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="116" t="s">
+      <c r="C52" s="92" t="s">
         <v>62</v>
       </c>
-      <c r="D52" s="117"/>
-      <c r="E52" s="110" t="s">
+      <c r="D52" s="93"/>
+      <c r="E52" s="94" t="s">
         <v>63</v>
       </c>
-      <c r="F52" s="111"/>
-      <c r="G52" s="111"/>
-      <c r="H52" s="112"/>
+      <c r="F52" s="95"/>
+      <c r="G52" s="95"/>
+      <c r="H52" s="96"/>
       <c r="L52" s="15"/>
       <c r="M52" s="19"/>
       <c r="N52" s="18"/>
@@ -6931,13 +6934,13 @@
       <c r="Q52" s="16"/>
     </row>
     <row r="53" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="114"/>
-      <c r="C53" s="116"/>
-      <c r="D53" s="117"/>
-      <c r="E53" s="110"/>
-      <c r="F53" s="111"/>
-      <c r="G53" s="111"/>
-      <c r="H53" s="112"/>
+      <c r="B53" s="90"/>
+      <c r="C53" s="92"/>
+      <c r="D53" s="93"/>
+      <c r="E53" s="94"/>
+      <c r="F53" s="95"/>
+      <c r="G53" s="95"/>
+      <c r="H53" s="96"/>
       <c r="L53" s="16"/>
       <c r="M53" s="16"/>
       <c r="N53" s="16"/>
@@ -6946,13 +6949,13 @@
       <c r="Q53" s="16"/>
     </row>
     <row r="54" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="114"/>
-      <c r="C54" s="116"/>
-      <c r="D54" s="117"/>
-      <c r="E54" s="110"/>
-      <c r="F54" s="111"/>
-      <c r="G54" s="111"/>
-      <c r="H54" s="112"/>
+      <c r="B54" s="90"/>
+      <c r="C54" s="92"/>
+      <c r="D54" s="93"/>
+      <c r="E54" s="94"/>
+      <c r="F54" s="95"/>
+      <c r="G54" s="95"/>
+      <c r="H54" s="96"/>
       <c r="L54" s="16"/>
       <c r="M54" s="16"/>
       <c r="N54" s="16"/>
@@ -6961,13 +6964,13 @@
       <c r="Q54" s="16"/>
     </row>
     <row r="55" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="114"/>
-      <c r="C55" s="116"/>
-      <c r="D55" s="117"/>
-      <c r="E55" s="110"/>
-      <c r="F55" s="111"/>
-      <c r="G55" s="111"/>
-      <c r="H55" s="112"/>
+      <c r="B55" s="90"/>
+      <c r="C55" s="92"/>
+      <c r="D55" s="93"/>
+      <c r="E55" s="94"/>
+      <c r="F55" s="95"/>
+      <c r="G55" s="95"/>
+      <c r="H55" s="96"/>
       <c r="L55" s="16"/>
       <c r="M55" s="16"/>
       <c r="N55" s="16"/>
@@ -6976,19 +6979,19 @@
       <c r="Q55" s="16"/>
     </row>
     <row r="56" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="113" t="s">
+      <c r="B56" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="C56" s="116" t="s">
+      <c r="C56" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="D56" s="117"/>
-      <c r="E56" s="110" t="s">
+      <c r="D56" s="93"/>
+      <c r="E56" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="F56" s="111"/>
-      <c r="G56" s="111"/>
-      <c r="H56" s="112"/>
+      <c r="F56" s="95"/>
+      <c r="G56" s="95"/>
+      <c r="H56" s="96"/>
       <c r="L56" s="15"/>
       <c r="M56" s="19"/>
       <c r="N56" s="18"/>
@@ -6997,13 +7000,13 @@
       <c r="Q56" s="16"/>
     </row>
     <row r="57" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="114"/>
-      <c r="C57" s="116"/>
-      <c r="D57" s="117"/>
-      <c r="E57" s="110"/>
-      <c r="F57" s="111"/>
-      <c r="G57" s="111"/>
-      <c r="H57" s="112"/>
+      <c r="B57" s="90"/>
+      <c r="C57" s="92"/>
+      <c r="D57" s="93"/>
+      <c r="E57" s="94"/>
+      <c r="F57" s="95"/>
+      <c r="G57" s="95"/>
+      <c r="H57" s="96"/>
       <c r="L57" s="16"/>
       <c r="M57" s="16"/>
       <c r="N57" s="16"/>
@@ -7012,13 +7015,13 @@
       <c r="Q57" s="16"/>
     </row>
     <row r="58" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="114"/>
-      <c r="C58" s="116"/>
-      <c r="D58" s="117"/>
-      <c r="E58" s="110"/>
-      <c r="F58" s="111"/>
-      <c r="G58" s="111"/>
-      <c r="H58" s="112"/>
+      <c r="B58" s="90"/>
+      <c r="C58" s="92"/>
+      <c r="D58" s="93"/>
+      <c r="E58" s="94"/>
+      <c r="F58" s="95"/>
+      <c r="G58" s="95"/>
+      <c r="H58" s="96"/>
       <c r="L58" s="16"/>
       <c r="M58" s="16"/>
       <c r="N58" s="16"/>
@@ -7027,13 +7030,13 @@
       <c r="Q58" s="16"/>
     </row>
     <row r="59" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="114"/>
-      <c r="C59" s="116"/>
-      <c r="D59" s="117"/>
-      <c r="E59" s="110"/>
-      <c r="F59" s="111"/>
-      <c r="G59" s="111"/>
-      <c r="H59" s="112"/>
+      <c r="B59" s="90"/>
+      <c r="C59" s="92"/>
+      <c r="D59" s="93"/>
+      <c r="E59" s="94"/>
+      <c r="F59" s="95"/>
+      <c r="G59" s="95"/>
+      <c r="H59" s="96"/>
       <c r="L59" s="16"/>
       <c r="M59" s="16"/>
       <c r="N59" s="16"/>
@@ -7042,19 +7045,19 @@
       <c r="Q59" s="16"/>
     </row>
     <row r="60" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="113" t="s">
+      <c r="B60" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="C60" s="116" t="s">
+      <c r="C60" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="D60" s="117"/>
-      <c r="E60" s="139" t="s">
+      <c r="D60" s="93"/>
+      <c r="E60" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="F60" s="140"/>
-      <c r="G60" s="140"/>
-      <c r="H60" s="141"/>
+      <c r="F60" s="100"/>
+      <c r="G60" s="100"/>
+      <c r="H60" s="101"/>
       <c r="L60" s="15"/>
       <c r="M60" s="19"/>
       <c r="N60" s="18"/>
@@ -7063,13 +7066,13 @@
       <c r="Q60" s="16"/>
     </row>
     <row r="61" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="114"/>
-      <c r="C61" s="116"/>
-      <c r="D61" s="117"/>
-      <c r="E61" s="142"/>
-      <c r="F61" s="143"/>
-      <c r="G61" s="143"/>
-      <c r="H61" s="144"/>
+      <c r="B61" s="90"/>
+      <c r="C61" s="92"/>
+      <c r="D61" s="93"/>
+      <c r="E61" s="102"/>
+      <c r="F61" s="103"/>
+      <c r="G61" s="103"/>
+      <c r="H61" s="104"/>
       <c r="L61" s="16"/>
       <c r="M61" s="16"/>
       <c r="N61" s="16"/>
@@ -7078,13 +7081,13 @@
       <c r="Q61" s="16"/>
     </row>
     <row r="62" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="114"/>
-      <c r="C62" s="116"/>
-      <c r="D62" s="117"/>
-      <c r="E62" s="142"/>
-      <c r="F62" s="143"/>
-      <c r="G62" s="143"/>
-      <c r="H62" s="144"/>
+      <c r="B62" s="90"/>
+      <c r="C62" s="92"/>
+      <c r="D62" s="93"/>
+      <c r="E62" s="102"/>
+      <c r="F62" s="103"/>
+      <c r="G62" s="103"/>
+      <c r="H62" s="104"/>
       <c r="L62" s="16"/>
       <c r="M62" s="16"/>
       <c r="N62" s="16"/>
@@ -7093,13 +7096,13 @@
       <c r="Q62" s="16"/>
     </row>
     <row r="63" spans="2:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="136"/>
-      <c r="C63" s="137"/>
-      <c r="D63" s="138"/>
-      <c r="E63" s="145"/>
-      <c r="F63" s="146"/>
-      <c r="G63" s="146"/>
-      <c r="H63" s="147"/>
+      <c r="B63" s="91"/>
+      <c r="C63" s="97"/>
+      <c r="D63" s="98"/>
+      <c r="E63" s="105"/>
+      <c r="F63" s="106"/>
+      <c r="G63" s="106"/>
+      <c r="H63" s="107"/>
       <c r="L63" s="16"/>
       <c r="M63" s="16"/>
       <c r="N63" s="16"/>
@@ -7237,12 +7240,26 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="C56:D59"/>
-    <mergeCell ref="E56:H59"/>
-    <mergeCell ref="C60:D63"/>
-    <mergeCell ref="E60:H63"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="C32:D35"/>
+    <mergeCell ref="E32:H35"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="C36:D39"/>
+    <mergeCell ref="E36:H39"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:D43"/>
+    <mergeCell ref="C44:D47"/>
+    <mergeCell ref="E40:H43"/>
+    <mergeCell ref="E44:H47"/>
+    <mergeCell ref="C48:D51"/>
+    <mergeCell ref="E48:H51"/>
+    <mergeCell ref="C52:D55"/>
+    <mergeCell ref="E52:H55"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="B48:B51"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C6:E6"/>
@@ -7258,26 +7275,12 @@
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C36:D39"/>
-    <mergeCell ref="E36:H39"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:D43"/>
-    <mergeCell ref="C44:D47"/>
-    <mergeCell ref="E40:H43"/>
-    <mergeCell ref="E44:H47"/>
-    <mergeCell ref="C48:D51"/>
-    <mergeCell ref="E48:H51"/>
-    <mergeCell ref="C52:D55"/>
-    <mergeCell ref="E52:H55"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="C32:D35"/>
-    <mergeCell ref="E32:H35"/>
-    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="C56:D59"/>
+    <mergeCell ref="E56:H59"/>
+    <mergeCell ref="C60:D63"/>
+    <mergeCell ref="E60:H63"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2:E2" r:id="rId1" display="Rokomari" xr:uid="{6274439F-671B-4149-AE4C-6FA6F68154E1}"/>

</xml_diff>